<commit_message>
first red box done
</commit_message>
<xml_diff>
--- a/Lab4/absExample-lab.xlsx
+++ b/Lab4/absExample-lab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Desktop\AI-in-the-wild\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB21549F-A96A-4D14-A26A-168B807EDE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29914B36-23CC-4526-92A3-460801AC5935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56DC7B23-590F-4E30-B993-F1A4F72C03A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{56DC7B23-590F-4E30-B993-F1A4F72C03A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hide" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>B</t>
   </si>
@@ -144,6 +144,15 @@
   <si>
     <t>A Protect Behaviour</t>
   </si>
+  <si>
+    <t>VectorA</t>
+  </si>
+  <si>
+    <t>VectorR</t>
+  </si>
+  <si>
+    <t>Sum product</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,6 +317,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -440,7 +450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58D1FDB0-1E94-473E-8CE3-F01B89FBE840}" type="CELLRANGE">
+                    <a:fld id="{A8644327-D051-4DEF-8F18-0AFAA61B73D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -449,7 +459,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{48EAB64A-5030-4DE3-BEF7-285CFB4E8B78}" type="XVALUE">
+                    <a:fld id="{FFDEEF7F-7B1B-400C-9B90-1FEFE91DEE10}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -458,7 +468,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{7322E320-276B-4BEF-B698-A7383D005C1E}" type="YVALUE">
+                    <a:fld id="{FF128276-A620-43B5-9640-03EA2A59934F}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -492,7 +502,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{055B3C78-B200-48AC-8616-70C8E47220F9}" type="CELLRANGE">
+                    <a:fld id="{589B3175-9554-4235-BCCD-450FD9E31530}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -501,7 +511,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{203EA555-CA1E-4A5A-B5B3-5A9A0907F997}" type="XVALUE">
+                    <a:fld id="{88602510-D4B1-4D5F-AB43-9CF9B8B5BCE3}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -510,7 +520,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{70F39356-6132-451B-86F9-88D9380F8249}" type="YVALUE">
+                    <a:fld id="{8EE9D6F4-43DE-4404-8FC0-702C1BF5C0F1}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -544,7 +554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A875088E-9DF1-4447-8E04-7E5121AFB24E}" type="CELLRANGE">
+                    <a:fld id="{3BA2A969-C7C6-4CC5-8CD3-CE71128295F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -553,7 +563,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{818A8EE8-0963-4FB8-8125-F5F5553B5401}" type="XVALUE">
+                    <a:fld id="{48153B9F-E83D-4CC2-909B-FB34C29903EA}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -562,7 +572,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{55C752CA-C7D1-4588-B3AD-2462363DD81F}" type="YVALUE">
+                    <a:fld id="{FA951373-6A68-4FE7-BB9E-13EA053208E4}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -596,7 +606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C224F81-441B-45ED-A6F6-3412D8D3B5CC}" type="CELLRANGE">
+                    <a:fld id="{B7FDF904-6735-4BF2-9B42-6573C2058A0D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -605,7 +615,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{F9F12B00-4C58-4235-A9AA-6173B784DF78}" type="XVALUE">
+                    <a:fld id="{078AD6B0-9C81-4B9C-BC1F-35C12BE725D0}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -614,7 +624,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{01F7677C-BA2B-4E1C-8E7A-22D0572DC60C}" type="YVALUE">
+                    <a:fld id="{5523E244-AD69-4FD5-B286-E37BBA02D48C}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1108,7 +1118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B2DB484-9EBD-4B33-8CCA-E17A2B4E9622}" type="CELLRANGE">
+                    <a:fld id="{2C4A1505-5F67-49DC-968A-BA6DD450073D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1117,7 +1127,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{0918D820-8BA4-4856-93D0-B6AA1BFAE187}" type="XVALUE">
+                    <a:fld id="{DAF1A8C8-CD99-4E78-988B-BF1F2E39D908}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1126,7 +1136,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{AC6EEEE6-36CF-4567-889C-BD31E9DC22E2}" type="YVALUE">
+                    <a:fld id="{8FBD7C04-DBBB-40A6-B406-860F6628CAD0}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1160,7 +1170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{272FCC1D-4403-4557-B576-DFA98AEC6CDB}" type="CELLRANGE">
+                    <a:fld id="{07518BD9-0AAF-4276-A51D-A2223F79EF83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1169,7 +1179,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{EEAEBDDA-A629-4F25-801E-3954254401F0}" type="XVALUE">
+                    <a:fld id="{85A09278-4828-44EC-B840-75C60D257F3A}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1178,7 +1188,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{EBAE1DC6-3B1E-4103-8616-0F17F0613107}" type="YVALUE">
+                    <a:fld id="{0F8AAD61-A4A2-40B2-8169-37B0C579D41D}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1212,7 +1222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08865958-DB18-46FC-8A76-07A7C9F0C4F3}" type="CELLRANGE">
+                    <a:fld id="{9F10A316-6701-4118-BFAE-F87C3AC33E31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1221,7 +1231,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{E17B34D5-3866-4A59-8DA6-05252B3B2F64}" type="XVALUE">
+                    <a:fld id="{006F6E1F-B183-4849-8486-AEDF44EC3395}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1230,7 +1240,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{2EFB3DD6-7AA0-493D-934B-33A8B38D5E2C}" type="YVALUE">
+                    <a:fld id="{75959D88-2ED4-449F-A9A8-2A289A726673}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1264,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{650F3130-2CB1-4BA1-8AF4-F59C633F66D8}" type="CELLRANGE">
+                    <a:fld id="{FD95E344-1EB3-4DC3-86E8-633751436B1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1273,7 +1283,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{292A4B88-2DAC-4BA4-99C4-2C3FBB2998F9}" type="XVALUE">
+                    <a:fld id="{C423FC33-4D9F-4799-BD3E-80D464BA41B1}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1282,7 +1292,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{23334D51-EE7E-4EC4-94A3-397616EFFFB4}" type="YVALUE">
+                    <a:fld id="{4C4540E9-91FD-4139-BE77-417E8B2BB137}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1316,7 +1326,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3A4137E-EB64-4B60-A269-B0DD72D9D755}" type="CELLRANGE">
+                    <a:fld id="{996ED2EC-1236-4368-A1D6-53690F52E535}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1325,7 +1335,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{7C4932E0-4E39-4A6D-BF54-9CE4CA2EB38D}" type="XVALUE">
+                    <a:fld id="{9C4AF4DF-00E2-4B99-9BA2-90E9426DC637}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1334,7 +1344,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{6810D966-0B00-4EA5-9A2D-B2EF0ABE17D0}" type="YVALUE">
+                    <a:fld id="{3BF0C11B-A9F5-4ACD-B3FE-8A78D6C0D53B}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1434,7 +1444,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>2.7</c:v>
+                  <c:v>2.7071067811865475</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
@@ -1458,7 +1468,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>2.7</c:v>
+                  <c:v>2.7071067811865475</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -3178,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FEE368-21E2-45D7-B375-E343DCEC543F}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,8 +3475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D4DD6-9DB9-4330-B473-8E9FCFE6A7A8}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,29 +3601,42 @@
       <c r="I14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="J14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="12">
+        <f>K13-K12</f>
+        <v>3</v>
+      </c>
+      <c r="L14" s="12">
+        <f>L13-L12</f>
+        <v>3</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="20" t="s">
         <v>4</v>
       </c>
       <c r="O14" s="7">
         <f>K18</f>
-        <v>2.7</v>
+        <v>2.7071067811865475</v>
       </c>
       <c r="P14" s="7">
         <f>L18</f>
-        <v>2.7</v>
+        <v>2.7071067811865475</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="6"/>
+      <c r="J15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="13">
+        <f>SQRT(K14*K14+L14*L14)</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="L15" s="14"/>
       <c r="M15" s="4" t="s">
         <v>22</v>
       </c>
@@ -3634,12 +3657,18 @@
       <c r="I16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
+      <c r="J16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="14">
+        <f>K14/K15</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="L16" s="14">
+        <f>L14/K15</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I17" s="4" t="s">
@@ -3651,9 +3680,18 @@
       <c r="K17" s="3">
         <v>1</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="16"/>
+      <c r="M17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" s="6">
+        <v>2</v>
+      </c>
+      <c r="P17" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I18" s="4" t="s">
@@ -3663,20 +3701,36 @@
         <v>4</v>
       </c>
       <c r="K18" s="21">
-        <v>2.7</v>
+        <f>K12+K16*K17</f>
+        <v>2.7071067811865475</v>
       </c>
       <c r="L18" s="21">
-        <v>2.7</v>
-      </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="16"/>
+        <f>L12+L16*K17</f>
+        <v>2.7071067811865475</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="6">
+        <v>5</v>
+      </c>
+      <c r="P18" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="M19" s="1"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="M19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="6">
+        <f>SUMPRODUCT(O17:P17, O18:P18)</f>
+        <v>16</v>
+      </c>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
       <c r="M20" s="4" t="s">
@@ -3739,6 +3793,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d71ff2ac-62c7-44d6-abd7-1383af8796a8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009908F051F1A7FA40B6E0D78DFA896E6F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22aea654b46515001aa88794d6829f47">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d71ff2ac-62c7-44d6-abd7-1383af8796a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dc07c26ce5bf35373bcca599f98562b8" ns3:_="">
     <xsd:import namespace="d71ff2ac-62c7-44d6-abd7-1383af8796a8"/>
@@ -3932,37 +4003,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d71ff2ac-62c7-44d6-abd7-1383af8796a8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C216F-E735-4F5C-923D-AD37EFD24405}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9786925A-CD28-47DD-B237-268CF7A5A0E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d71ff2ac-62c7-44d6-abd7-1383af8796a8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3984,9 +4028,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9786925A-CD28-47DD-B237-268CF7A5A0E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C20C216F-E735-4F5C-923D-AD37EFD24405}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d71ff2ac-62c7-44d6-abd7-1383af8796a8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>